<commit_message>
Atualizações de status e de arquivos
</commit_message>
<xml_diff>
--- a/02-Projeto/01-ResolveAi/02-GQA/01-AuditoriaGRE/01-Auditoria/03-ChecklistGQA.xlsx
+++ b/02-Projeto/01-ResolveAi/02-GQA/01-AuditoriaGRE/01-Auditoria/03-ChecklistGQA.xlsx
@@ -99,10 +99,7 @@
     <t>Observação</t>
   </si>
   <si>
-    <t>O uso da síntaxe UML está correto?</t>
-  </si>
-  <si>
-    <t>Todas as relacões possuem nome?</t>
+    <t>O uso da sintaxe UML está correto?</t>
   </si>
   <si>
     <t>A notação do diagrama de  caso de uso foi utilizada de forma adequada?</t>
@@ -111,13 +108,22 @@
     <t>Os nomes dos atores referenciados no caso de uso denotam claramente o papel que estes desempenham?</t>
   </si>
   <si>
+    <t>O protótipo contempla todos os perfis de usuários do sistema?</t>
+  </si>
+  <si>
     <t>As interações e trocas de informações e mensagens entre ator e sistema estão claras?</t>
   </si>
   <si>
-    <t>O caso de uso está descrito de forma clara, intuitiva e sem ambiguidade?</t>
+    <t>Todas as relações possuem nome?</t>
   </si>
   <si>
     <t>O documento segue as normas gramaticais e ortográficas da língua portuguesa?</t>
+  </si>
+  <si>
+    <t>Todas as telas do protótipo tem uma identificação de contexto explícita, na parte superior, para o usuário dos sistema?</t>
+  </si>
+  <si>
+    <t>O protótipo segue as normas gramaticais e ortográficas da língua portuguesa?</t>
   </si>
   <si>
     <t>Todas as relações tem suas multiplicidades indicadas?</t>
@@ -127,12 +133,6 @@
   </si>
   <si>
     <t>Todos os atributos começam com letras minúsculas?</t>
-  </si>
-  <si>
-    <t>Todos os requisitos estão sendo atendidos no protótipo?</t>
-  </si>
-  <si>
-    <t>O protótipo segue as normas gramaticais e ortográficas da língua portuguesa?</t>
   </si>
   <si>
     <t>Lista de Inconformidades</t>
@@ -193,6 +193,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="12.0"/>
     </font>
@@ -200,13 +201,12 @@
       <b/>
       <sz val="12.0"/>
     </font>
-    <font/>
+    <font>
+      <b/>
+    </font>
     <font>
       <b/>
       <sz val="18.0"/>
-    </font>
-    <font>
-      <b/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -382,33 +382,33 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -433,8 +433,8 @@
     <xf borderId="8" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -505,45 +505,45 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -551,7 +551,7 @@
       <c r="F8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -574,7 +574,7 @@
         <v>1.0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="19"/>
@@ -586,7 +586,7 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -610,23 +610,11 @@
         <v>4.0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -650,55 +638,55 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8">
@@ -741,7 +729,7 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -752,7 +740,7 @@
         <v>3.0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -763,7 +751,7 @@
         <v>4.0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -774,7 +762,7 @@
         <v>5.0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -809,59 +797,59 @@
     <col customWidth="1" min="1" max="1" width="6.29"/>
     <col customWidth="1" min="2" max="2" width="6.43"/>
     <col customWidth="1" min="3" max="3" width="35.57"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
+    <col customWidth="1" min="5" max="5" width="26.29"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8">
@@ -893,7 +881,7 @@
         <v>1.0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="19"/>
@@ -904,11 +892,22 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>